<commit_message>
player list, get from template.xlsx
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Local Sites/playhq-puppeteer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ADA7B4-DFBC-6C4B-80F8-9BF80CBF3B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9A787B9-DEC9-A548-9E26-4F4F6FA2E88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19360" windowHeight="17420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="30000" windowHeight="17720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keyborough 2 (Grading)" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +162,36 @@
   </si>
   <si>
     <t>Rebound (Defensive)</t>
+  </si>
+  <si>
+    <t>Hugo Fischer</t>
+  </si>
+  <si>
+    <t>Leo Robbins</t>
+  </si>
+  <si>
+    <t>Nate Harrison</t>
+  </si>
+  <si>
+    <t>Thomas Semple</t>
+  </si>
+  <si>
+    <t>Zacharie Khan</t>
+  </si>
+  <si>
+    <t>Harrison Bradley</t>
+  </si>
+  <si>
+    <t>Zakk Bosman</t>
+  </si>
+  <si>
+    <t>Harley Stein</t>
+  </si>
+  <si>
+    <t>Charles Ferro</t>
+  </si>
+  <si>
+    <t>Heath Curtis</t>
   </si>
   <si>
     <t>#</t>
@@ -317,327 +349,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -672,6 +383,44 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -782,6 +531,120 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -797,7 +660,64 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -846,6 +766,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -861,22 +800,79 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -903,6 +899,42 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1844,55 +1876,55 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0A5F5190-7923-AA47-94BD-06EB5CE9D4CF}" name="Table15" displayName="Table15" ref="A1:R19" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36">
-  <autoFilter ref="A1:R18" xr:uid="{9289FB7A-F9FE-47B2-A61A-372F1EAF4D76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0A5F5190-7923-AA47-94BD-06EB5CE9D4CF}" name="Table15" displayName="Table15" ref="A1:R12" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36">
+  <autoFilter ref="A1:R11" xr:uid="{9289FB7A-F9FE-47B2-A61A-372F1EAF4D76}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{62D4EE4D-C20B-864B-9187-DDCFE82FE18B}" name="#" totalsRowLabel="TOTAL" dataDxfId="35" totalsRowDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{8D5F1A19-007B-7147-AF72-3693ED107653}" name="Name" dataDxfId="34" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{AFEC4163-23CE-794F-8411-5EBE02F3314C}" name="Steals" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="15">
+    <tableColumn id="1" xr3:uid="{62D4EE4D-C20B-864B-9187-DDCFE82FE18B}" name="#" totalsRowLabel="TOTAL" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{8D5F1A19-007B-7147-AF72-3693ED107653}" name="Name" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{AFEC4163-23CE-794F-8411-5EBE02F3314C}" name="Steals" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
       <totalsRowFormula>SUM(Table15[Steals])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{55C71104-A5CC-5B4A-85AD-CDDDFFFC9E0B}" name="Turnovers" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="14">
+    <tableColumn id="3" xr3:uid="{55C71104-A5CC-5B4A-85AD-CDDDFFFC9E0B}" name="Turnovers" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <totalsRowFormula>SUM(Table15[Turnovers])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0A5F08E2-08E5-224B-8899-3BAA76F29F03}" name="Assists" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="13">
+    <tableColumn id="4" xr3:uid="{0A5F08E2-08E5-224B-8899-3BAA76F29F03}" name="Assists" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
       <totalsRowFormula>SUM(Table15[Assists])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4637DF51-6285-274D-AE77-A78C08833436}" name="Rebound (Offensive)" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="12">
+    <tableColumn id="5" xr3:uid="{4637DF51-6285-274D-AE77-A78C08833436}" name="Rebound (Offensive)" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
       <totalsRowFormula>SUM(Table15[Rebound (Offensive)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F5E9E444-BC58-F240-953D-4F06EEDC88E8}" name="Rebound (Defensive)" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="11">
+    <tableColumn id="6" xr3:uid="{F5E9E444-BC58-F240-953D-4F06EEDC88E8}" name="Rebound (Defensive)" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUM(Table15[Rebound (Defensive)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{4D352443-4EDA-844C-8833-71848E9987A7}" name="Charge (Offensive)" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="10">
+    <tableColumn id="12" xr3:uid="{4D352443-4EDA-844C-8833-71848E9987A7}" name="Charge (Offensive)" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUM(Table15[Charge (Offensive)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BDA422A5-F0F2-E347-8342-676DF7B0AE26}" name="Charge (Defensive)" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="9">
+    <tableColumn id="9" xr3:uid="{BDA422A5-F0F2-E347-8342-676DF7B0AE26}" name="Charge (Defensive)" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUM(Table15[Charge (Defensive)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{71017EB4-69AC-CC43-9505-3DCF1281384D}" name="Field Goal (A)" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="8">
+    <tableColumn id="7" xr3:uid="{71017EB4-69AC-CC43-9505-3DCF1281384D}" name="Field Goal (A)" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUM(Table15[Field Goal (A)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7A81D1F6-F704-CB47-A5C6-32B2A8CC83BD}" name="Three Pointer (A)" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="7">
+    <tableColumn id="13" xr3:uid="{7A81D1F6-F704-CB47-A5C6-32B2A8CC83BD}" name="Three Pointer (A)" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUM(Table15[Three Pointer (A)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C9C5C64D-B6D2-0F43-B742-81C7D92AD0D7}" name="Foul Shot (A)" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="6">
+    <tableColumn id="11" xr3:uid="{C9C5C64D-B6D2-0F43-B742-81C7D92AD0D7}" name="Foul Shot (A)" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUM(Table15[Foul Shot (A)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{BCB58A41-91E6-D644-8402-3BEE1D301972}" name="Field Goal (M)" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="5">
+    <tableColumn id="14" xr3:uid="{BCB58A41-91E6-D644-8402-3BEE1D301972}" name="Field Goal (M)" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table15[Field Goal (M)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{3427C1D8-11B9-C448-8CFC-73CBE605A5BD}" name="Three Pointer (M)" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="4">
+    <tableColumn id="15" xr3:uid="{3427C1D8-11B9-C448-8CFC-73CBE605A5BD}" name="Three Pointer (M)" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Table15[Three Pointer (M)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9485E5E0-7533-B04C-BA17-A3336F51A3F7}" name="Foul Shot (M)" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{9485E5E0-7533-B04C-BA17-A3336F51A3F7}" name="Foul Shot (M)" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Table15[Foul Shot (M)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5A66CC86-7A2A-F946-9EB5-BE2F1815C28E}" name="Points " totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{5A66CC86-7A2A-F946-9EB5-BE2F1815C28E}" name="Points " totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table15[[Points ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{770C0366-2674-CE42-9626-8FC9CBE2DD4A}" name="Fouls" dataDxfId="19" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{6C63BB21-597E-DE46-8756-211705B4DCC1}" name="Notes" dataDxfId="18" totalsRowDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{770C0366-2674-CE42-9626-8FC9CBE2DD4A}" name="Fouls" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{6C63BB21-597E-DE46-8756-211705B4DCC1}" name="Notes" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2848,7 +2880,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3270,10 +3302,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2AB1E3-EB5C-844B-B436-311A4E55F778}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="P1" activeCellId="2" sqref="M1:O1 Q1 P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -3297,7 +3329,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3345,7 +3377,7 @@
         <v>7</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>30</v>
@@ -3353,6 +3385,12 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -3372,6 +3410,12 @@
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3391,6 +3435,12 @@
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3410,6 +3460,12 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3429,6 +3485,12 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -3448,6 +3510,12 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -3467,6 +3535,12 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -3486,6 +3560,12 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -3505,6 +3585,12 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3523,7 +3609,13 @@
       <c r="R10" s="5"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -3542,225 +3634,92 @@
       <c r="R11" s="5"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="5">
+        <f>SUM(Table15[Steals])</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <f>SUM(Table15[Turnovers])</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <f>SUM(Table15[Assists])</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <f>SUM(Table15[Rebound (Offensive)])</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <f>SUM(Table15[Rebound (Defensive)])</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <f>SUM(Table15[Charge (Offensive)])</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>SUM(Table15[Charge (Defensive)])</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <f>SUM(Table15[Field Goal (A)])</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <f>SUM(Table15[Three Pointer (A)])</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
+        <f>SUM(Table15[Foul Shot (A)])</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <f>SUM(Table15[Field Goal (M)])</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <f>SUM(Table15[Three Pointer (M)])</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <f>SUM(Table15[Foul Shot (M)])</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <f>SUM(Table15[[Points ]])</f>
+        <v>0</v>
+      </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="5">
-        <f>SUM(Table15[Steals])</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <f>SUM(Table15[Turnovers])</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <f>SUM(Table15[Assists])</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <f>SUM(Table15[Rebound (Offensive)])</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
-        <f>SUM(Table15[Rebound (Defensive)])</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <f>SUM(Table15[Charge (Offensive)])</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <f>SUM(Table15[Charge (Defensive)])</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <f>SUM(Table15[Field Goal (A)])</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <f>SUM(Table15[Three Pointer (A)])</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
-        <f>SUM(Table15[Foul Shot (A)])</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="5">
-        <f>SUM(Table15[Field Goal (M)])</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="5">
-        <f>SUM(Table15[Three Pointer (M)])</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="5">
-        <f>SUM(Table15[Foul Shot (M)])</f>
-        <v>0</v>
-      </c>
-      <c r="P19" s="5">
-        <f>SUM(Table15[[Points ]])</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:19" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="9"/>
+    <row r="13" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:19" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>